<commit_message>
Log + persoonlijk dossier + maps filmpje
</commit_message>
<xml_diff>
--- a/Doc/Logboeken/Yousfi_Log.xlsx
+++ b/Doc/Logboeken/Yousfi_Log.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="75">
   <si>
     <t>datum</t>
   </si>
@@ -135,6 +135,114 @@
   </si>
   <si>
     <t>6 uur</t>
+  </si>
+  <si>
+    <t>3 March</t>
+  </si>
+  <si>
+    <t>4 March</t>
+  </si>
+  <si>
+    <t>3 uur</t>
+  </si>
+  <si>
+    <t>5 March</t>
+  </si>
+  <si>
+    <t>6 March</t>
+  </si>
+  <si>
+    <t>7 March</t>
+  </si>
+  <si>
+    <t>8 March</t>
+  </si>
+  <si>
+    <t>Map wijziging (-&gt; gelimiteerd tot 1 globale variabele)</t>
+  </si>
+  <si>
+    <t>Dropdown Geolocation gefixt</t>
+  </si>
+  <si>
+    <t>Debugging</t>
+  </si>
+  <si>
+    <t>Database wijzigingen (foreign keys)</t>
+  </si>
+  <si>
+    <t>Extra maps functie toegevoegd (getCoordinates())</t>
+  </si>
+  <si>
+    <t>Debugging/refactoring</t>
+  </si>
+  <si>
+    <t>9 March</t>
+  </si>
+  <si>
+    <t>Tekst meldingen bij text areas weg</t>
+  </si>
+  <si>
+    <t>14 March</t>
+  </si>
+  <si>
+    <t>Oman logo verfijnd</t>
+  </si>
+  <si>
+    <t>21 March</t>
+  </si>
+  <si>
+    <t>Map required gemaakt</t>
+  </si>
+  <si>
+    <t>23 March</t>
+  </si>
+  <si>
+    <t>Kleine servgeolocation wijziging</t>
+  </si>
+  <si>
+    <t>Validatie/opmaak/efficientie</t>
+  </si>
+  <si>
+    <t>25 March</t>
+  </si>
+  <si>
+    <t>26 March</t>
+  </si>
+  <si>
+    <t>Regex validatie op service-side</t>
+  </si>
+  <si>
+    <t>27 March</t>
+  </si>
+  <si>
+    <t>Validatie verfijning</t>
+  </si>
+  <si>
+    <t>2 May</t>
+  </si>
+  <si>
+    <t>Oplossing (algemeen dossier)</t>
+  </si>
+  <si>
+    <t>18 May</t>
+  </si>
+  <si>
+    <t>Sprint verslag</t>
+  </si>
+  <si>
+    <t>24 May</t>
+  </si>
+  <si>
+    <t>25 May</t>
+  </si>
+  <si>
+    <t>Persoonlijk dossier</t>
+  </si>
+  <si>
+    <t>26 May</t>
+  </si>
+  <si>
+    <t>Maps filmpje</t>
   </si>
 </sst>
 </file>
@@ -950,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1176,154 +1284,316 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="10"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="10"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="10"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="10"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="10"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="10"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="10"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="10"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="10"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="10"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="10"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="10"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="10"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="10"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="3"/>
-    </row>
-    <row r="35" spans="1:3">
+    <row r="17" spans="1:4">
+      <c r="A17" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="10"/>
       <c r="B35" s="2"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:4">
       <c r="A36" s="10"/>
       <c r="B36" s="2"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:4">
       <c r="A37" s="10"/>
       <c r="B37" s="2"/>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:4">
       <c r="A38" s="10"/>
       <c r="B38" s="2"/>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:4">
       <c r="A39" s="10"/>
       <c r="B39" s="2"/>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:4">
       <c r="B40" s="2"/>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:4">
       <c r="B41" s="2"/>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:4">
       <c r="B42" s="2"/>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:4">
       <c r="B43" s="2"/>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:4">
       <c r="B44" s="2"/>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:4">
       <c r="B45" s="2"/>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:4">
       <c r="B46" s="2"/>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:4">
       <c r="B47" s="2"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:4">
       <c r="B48" s="2"/>
       <c r="C48" s="3"/>
     </row>

</xml_diff>